<commit_message>
Auth, login and fetch proposals
</commit_message>
<xml_diff>
--- a/database tables/Database structure for ees applications..xlsx
+++ b/database tables/Database structure for ees applications..xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\apis.eesapplications\database tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4392B35D-6722-40C7-8D3D-C3C996DF9421}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC904A57-59E9-47F5-917C-92F99FB3941F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{BAD1A830-4027-43C3-8841-BC26DD6060E1}"/>
   </bookViews>
@@ -55,12 +55,37 @@
         </r>
       </text>
     </comment>
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{A8134EE3-A421-4781-B577-93844C67BC33}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Boppana Sandeep:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+As defined
+1</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
   <si>
     <t>ees applications</t>
   </si>
@@ -117,6 +142,18 @@
   </si>
   <si>
     <t>AI, Primary key</t>
+  </si>
+  <si>
+    <t>eesalogin</t>
+  </si>
+  <si>
+    <t>eesaId</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -208,12 +245,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -530,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A14C4D-501F-4CDA-B97E-B1433C341E5D}">
-  <dimension ref="B1:G12"/>
+  <dimension ref="B1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,112 +578,188 @@
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D1" s="4" t="s">
+    <row r="1" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="F4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="F5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="D6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="D7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="D8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="D9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="D10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+      <c r="D11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>